<commit_message>
Changing the sign from + to - for the material recycled for each component
</commit_message>
<xml_diff>
--- a/Recycling/Met_rec_comp/metrec_Avg_b1.xlsx
+++ b/Recycling/Met_rec_comp/metrec_Avg_b1.xlsx
@@ -618,7 +618,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>1.11281977126873E-06</v>
+        <v>-1.11281977126873E-06</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -649,16 +649,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>0.0004203312709097974</v>
+        <v>-0.0004203312709097974</v>
       </c>
       <c r="C4">
-        <v>3.23337081060437E-06</v>
+        <v>-3.23337081060437E-06</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>6677.182187102788</v>
+        <v>-6677.182187102788</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -672,7 +672,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>3715.204687041987</v>
+        <v>-3715.204687041987</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -713,7 +713,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>376433.009481501</v>
+        <v>-376433.009481501</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -744,16 +744,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>6718372.964071271</v>
+        <v>-6718372.964071271</v>
       </c>
       <c r="C4">
-        <v>1093750.790945931</v>
+        <v>-1093750.790945931</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>268154335.7213635</v>
+        <v>-268154335.7213635</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -767,7 +767,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>116767254.1413231</v>
+        <v>-116767254.1413231</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -808,7 +808,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>402496.1857895394</v>
+        <v>-402496.1857895394</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -839,16 +839,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>7157998.276420192</v>
+        <v>-7157998.276420192</v>
       </c>
       <c r="C4">
-        <v>1169479.058614979</v>
+        <v>-1169479.058614979</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>271116105.1008989</v>
+        <v>-271116105.1008989</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -862,7 +862,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>116273505.8214616</v>
+        <v>-116273505.8214616</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -903,7 +903,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>1.867980745206815E-05</v>
+        <v>-1.867980745206815E-05</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -934,16 +934,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>0.005906348838781798</v>
+        <v>-0.005906348838781798</v>
       </c>
       <c r="C4">
-        <v>5.427540534651564E-05</v>
+        <v>-5.427540534651564E-05</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>14795.29488720856</v>
+        <v>-14795.29488720856</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -957,7 +957,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>8232.127058941762</v>
+        <v>-8232.127058941762</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -998,7 +998,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0.0002336262700404519</v>
+        <v>-0.0002336262700404519</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1029,16 +1029,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>0.06284195190714177</v>
+        <v>-0.06284195190714177</v>
       </c>
       <c r="C4">
-        <v>0.0006788164459712436</v>
+        <v>-0.0006788164459712436</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>30794.52319715452</v>
+        <v>-30794.52319715452</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1052,7 +1052,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>17133.91621066002</v>
+        <v>-17133.91621066002</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1093,7 +1093,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0.002290942924124273</v>
+        <v>-0.002290942924124273</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1124,16 +1124,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>0.5338070722339813</v>
+        <v>-0.5338070722339813</v>
       </c>
       <c r="C4">
-        <v>0.006656484878210571</v>
+        <v>-0.006656484878210571</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>61227.42076098199</v>
+        <v>-61227.42076098199</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1147,7 +1147,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>34064.93595272944</v>
+        <v>-34064.93595272944</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1188,7 +1188,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0.01832686926551903</v>
+        <v>-0.01832686926551903</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1219,16 +1219,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>3.764592109082937</v>
+        <v>-3.764592109082937</v>
       </c>
       <c r="C4">
-        <v>0.05324992030410442</v>
+        <v>-0.05324992030410442</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>117643.4372118148</v>
+        <v>-117643.4372118148</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1242,7 +1242,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>65441.62116389273</v>
+        <v>-65441.62116389273</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1283,7 +1283,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0.1234080586389146</v>
+        <v>-0.1234080586389146</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1314,16 +1314,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>22.7074574445241</v>
+        <v>-22.7074574445241</v>
       </c>
       <c r="C4">
-        <v>0.3585702059745849</v>
+        <v>-0.3585702059745849</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>219719.4516099411</v>
+        <v>-219719.4516099411</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1337,7 +1337,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>122158.4899530898</v>
+        <v>-122158.4899530898</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1378,7 +1378,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0.7171912905329547</v>
+        <v>-0.7171912905329547</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1409,16 +1409,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>119.8907489117425</v>
+        <v>-119.8907489117425</v>
       </c>
       <c r="C4">
-        <v>2.083846319323655</v>
+        <v>-2.083846319323655</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>398738.89430813</v>
+        <v>-398738.89430813</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1432,7 +1432,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>221361.6989563337</v>
+        <v>-221361.6989563337</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1473,7 +1473,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>3.670480842135094</v>
+        <v>-3.670480842135094</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1504,16 +1504,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>564.3320657591172</v>
+        <v>-564.3320657591172</v>
       </c>
       <c r="C4">
-        <v>10.66482275230551</v>
+        <v>-10.66482275230551</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>701390.3364379051</v>
+        <v>-701390.3364379051</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1527,7 +1527,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>387908.0718825551</v>
+        <v>-387908.0718825551</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1568,7 +1568,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>16.81681533536907</v>
+        <v>-16.81681533536907</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1599,16 +1599,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>2403.298330474134</v>
+        <v>-2403.298330474134</v>
       </c>
       <c r="C4">
-        <v>48.86235959908689</v>
+        <v>-48.86235959908689</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>1196019.476201</v>
+        <v>-1196019.476201</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1622,7 +1622,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>655454.5607293999</v>
+        <v>-655454.5607293999</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1663,7 +1663,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>69.90889800994165</v>
+        <v>-69.90889800994165</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1694,16 +1694,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>9369.497122916056</v>
+        <v>-9369.497122916056</v>
       </c>
       <c r="C4">
-        <v>203.1248869429707</v>
+        <v>-203.1248869429707</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>1988270.072915811</v>
+        <v>-1988270.072915811</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1717,7 +1717,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>1067178.371186058</v>
+        <v>-1067178.371186058</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1853,7 +1853,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>266.5505796531776</v>
+        <v>-266.5505796531776</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1884,16 +1884,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>33737.49366855784</v>
+        <v>-33737.49366855784</v>
       </c>
       <c r="C4">
-        <v>774.4801863267161</v>
+        <v>-774.4801863267161</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>3265650.502312439</v>
+        <v>-3265650.502312439</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1907,7 +1907,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>1676022.387872362</v>
+        <v>-1676022.387872362</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1948,7 +1948,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>939.5126390310344</v>
+        <v>-939.5126390310344</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1979,16 +1979,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>112740.634666146</v>
+        <v>-112740.634666146</v>
       </c>
       <c r="C4">
-        <v>2729.815574514306</v>
+        <v>-2729.815574514306</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>5420730.855107742</v>
+        <v>-5420730.855107742</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2002,7 +2002,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>2544287.407847164</v>
+        <v>-2544287.407847164</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -2043,7 +2043,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>3070.97631213468</v>
+        <v>-3070.97631213468</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -2074,16 +2074,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>348499.3745080646</v>
+        <v>-348499.3745080646</v>
       </c>
       <c r="C4">
-        <v>8922.923032175235</v>
+        <v>-8922.923032175235</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>9351315.744038306</v>
+        <v>-9351315.744038306</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2097,7 +2097,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>3742368.092132013</v>
+        <v>-3742368.092132013</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -2138,7 +2138,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>9246.589093318147</v>
+        <v>-9246.589093318147</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -2169,16 +2169,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>975307.9847518718</v>
+        <v>-975307.9847518718</v>
       </c>
       <c r="C4">
-        <v>26866.57088946327</v>
+        <v>-26866.57088946327</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>16971792.99242272</v>
+        <v>-16971792.99242272</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2192,7 +2192,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>5346370.7073994</v>
+        <v>-5346370.7073994</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -2233,7 +2233,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>24918.96757844782</v>
+        <v>-24918.96757844782</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -2264,16 +2264,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>2327113.088246528</v>
+        <v>-2327113.088246528</v>
       </c>
       <c r="C4">
-        <v>72403.69418193308</v>
+        <v>-72403.69418193308</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>30998683.04348751</v>
+        <v>-30998683.04348751</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2287,7 +2287,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>7434218.633645034</v>
+        <v>-7434218.633645034</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -2328,7 +2328,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>55889.88068242896</v>
+        <v>-55889.88068242896</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -2359,16 +2359,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>4217764.771126897</v>
+        <v>-4217764.771126897</v>
       </c>
       <c r="C4">
-        <v>162391.7129012685</v>
+        <v>-162391.7129012685</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>50342860.6905093</v>
+        <v>-50342860.6905093</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2382,7 +2382,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>10079884.52484072</v>
+        <v>-10079884.52484072</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -2423,7 +2423,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>90728.50532815</v>
+        <v>-90728.50532815</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -2454,16 +2454,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>5346403.316659183</v>
+        <v>-5346403.316659183</v>
       </c>
       <c r="C4">
-        <v>263617.6211026011</v>
+        <v>-263617.6211026011</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>65317757.28481049</v>
+        <v>-65317757.28481049</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2477,7 +2477,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>13345846.92613791</v>
+        <v>-13345846.92613791</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -2518,7 +2518,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>89412.2970418473</v>
+        <v>-89412.2970418473</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -2549,16 +2549,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>5618402.989328753</v>
+        <v>-5618402.989328753</v>
       </c>
       <c r="C4">
-        <v>259793.2916258209</v>
+        <v>-259793.2916258209</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>74338057.62872626</v>
+        <v>-74338057.62872626</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2572,7 +2572,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>17274718.67509378</v>
+        <v>-17274718.67509378</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -2613,7 +2613,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>54500.67873856903</v>
+        <v>-54500.67873856903</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -2644,16 +2644,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>6061935.549912537</v>
+        <v>-6061935.549912537</v>
       </c>
       <c r="C4">
-        <v>158355.2955664197</v>
+        <v>-158355.2955664197</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>85016515.45118837</v>
+        <v>-85016515.45118837</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2667,7 +2667,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>21880277.29404883</v>
+        <v>-21880277.29404883</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -2708,7 +2708,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>48255.476636728</v>
+        <v>-48255.476636728</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -2739,16 +2739,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>6644858.215068342</v>
+        <v>-6644858.215068342</v>
       </c>
       <c r="C4">
-        <v>140209.4513751401</v>
+        <v>-140209.4513751401</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>98583636.54535446</v>
+        <v>-98583636.54535446</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2762,7 +2762,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>27139118.44363695</v>
+        <v>-27139118.44363695</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -2843,7 +2843,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0.05254526433966906</v>
+        <v>-0.05254526433966906</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2857,7 +2857,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>0.02923636013320883</v>
+        <v>-0.02923636013320883</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -2898,7 +2898,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>82210.39976254321</v>
+        <v>-82210.39976254321</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -2929,16 +2929,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>7295349.497927143</v>
+        <v>-7295349.497927143</v>
       </c>
       <c r="C4">
-        <v>238867.7068679909</v>
+        <v>-238867.7068679909</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>114677714.6194437</v>
+        <v>-114677714.6194437</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2952,7 +2952,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>32987083.62506209</v>
+        <v>-32987083.62506209</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -2993,7 +2993,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>122834.889734973</v>
+        <v>-122834.889734973</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -3024,16 +3024,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>7923241.120187508</v>
+        <v>-7923241.120187508</v>
       </c>
       <c r="C4">
-        <v>356904.8261427385</v>
+        <v>-356904.8261427385</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>131644420.782093</v>
+        <v>-131644420.782093</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -3047,7 +3047,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>39322753.23429316</v>
+        <v>-39322753.23429316</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -3088,7 +3088,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>173893.5042689031</v>
+        <v>-173893.5042689031</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -3119,16 +3119,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>8431188.034675952</v>
+        <v>-8431188.034675952</v>
       </c>
       <c r="C4">
-        <v>505258.9784738823</v>
+        <v>-505258.9784738823</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>148635385.2167982</v>
+        <v>-148635385.2167982</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -3142,7 +3142,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>46019827.39435996</v>
+        <v>-46019827.39435996</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -3183,7 +3183,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>234330.2277346166</v>
+        <v>-234330.2277346166</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -3214,16 +3214,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>8973043.306489497</v>
+        <v>-8973043.306489497</v>
       </c>
       <c r="C4">
-        <v>680861.8412086212</v>
+        <v>-680861.8412086212</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>166523427.9955721</v>
+        <v>-166523427.9955721</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -3237,7 +3237,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>52951569.30788335</v>
+        <v>-52951569.30788335</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -3278,7 +3278,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>269625.4017860388</v>
+        <v>-269625.4017860388</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -3309,16 +3309,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>8840141.125489665</v>
+        <v>-8840141.125489665</v>
       </c>
       <c r="C4">
-        <v>783414.2836431746</v>
+        <v>-783414.2836431746</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>179127594.7295502</v>
+        <v>-179127594.7295502</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -3332,7 +3332,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>60030249.43067586</v>
+        <v>-60030249.43067586</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -3373,7 +3373,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>314521.7720552256</v>
+        <v>-314521.7720552256</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -3404,16 +3404,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>8594333.838329772</v>
+        <v>-8594333.838329772</v>
       </c>
       <c r="C4">
-        <v>913863.6312180916</v>
+        <v>-913863.6312180916</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>191414007.1077119</v>
+        <v>-191414007.1077119</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -3427,7 +3427,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>67262590.15956321</v>
+        <v>-67262590.15956321</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -3468,7 +3468,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>484320.4076755798</v>
+        <v>-484320.4076755798</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -3499,16 +3499,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>8592747.242896536</v>
+        <v>-8592747.242896536</v>
       </c>
       <c r="C4">
-        <v>1407224.700341943</v>
+        <v>-1407224.700341943</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>209094778.6832773</v>
+        <v>-209094778.6832773</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -3522,7 +3522,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>74818673.10377096</v>
+        <v>-74818673.10377096</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -3563,7 +3563,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>757507.1937945902</v>
+        <v>-757507.1937945902</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -3594,16 +3594,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>8428565.98618944</v>
+        <v>-8428565.98618944</v>
       </c>
       <c r="C4">
-        <v>2200986.819676827</v>
+        <v>-2200986.819676827</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>229404078.953139</v>
+        <v>-229404078.953139</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -3617,7 +3617,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>83106342.42769842</v>
+        <v>-83106342.42769842</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -3658,7 +3658,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>1034378.602881528</v>
+        <v>-1034378.602881528</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -3689,16 +3689,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>8419129.865640102</v>
+        <v>-8419129.865640102</v>
       </c>
       <c r="C4">
-        <v>3005454.852637773</v>
+        <v>-3005454.852637773</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>253528250.863023</v>
+        <v>-253528250.863023</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -3712,7 +3712,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>92836729.44178124</v>
+        <v>-92836729.44178124</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -3753,7 +3753,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>1291207.258274031</v>
+        <v>-1291207.258274031</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -3784,16 +3784,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>8244922.311412376</v>
+        <v>-8244922.311412376</v>
       </c>
       <c r="C4">
-        <v>3751687.350579576</v>
+        <v>-3751687.350579576</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>280441992.9113191</v>
+        <v>-280441992.9113191</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -3807,7 +3807,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>105060390.9927068</v>
+        <v>-105060390.9927068</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -3888,7 +3888,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>2.210493821417531</v>
+        <v>-2.210493821417531</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -3902,7 +3902,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>1.229926126499775</v>
+        <v>-1.229926126499775</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -3943,7 +3943,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>1240057.032409812</v>
+        <v>-1240057.032409812</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -3974,16 +3974,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>7865910.251693619</v>
+        <v>-7865910.251693619</v>
       </c>
       <c r="C4">
-        <v>3603067.015521519</v>
+        <v>-3603067.015521519</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>305346968.4819759</v>
+        <v>-305346968.4819759</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -3997,7 +3997,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>121150471.2581205</v>
+        <v>-121150471.2581205</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -4038,7 +4038,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>1117622.001980129</v>
+        <v>-1117622.001980129</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -4069,16 +4069,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>7326764.169726046</v>
+        <v>-7326764.169726046</v>
       </c>
       <c r="C4">
-        <v>3247324.006808209</v>
+        <v>-3247324.006808209</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>337198045.2574171</v>
+        <v>-337198045.2574171</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -4092,7 +4092,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>142718128.0781966</v>
+        <v>-142718128.0781966</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -4133,7 +4133,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>1092950.5714229</v>
+        <v>-1092950.5714229</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -4164,16 +4164,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>6712633.183928545</v>
+        <v>-6712633.183928545</v>
       </c>
       <c r="C4">
-        <v>3175639.547671894</v>
+        <v>-3175639.547671894</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>383760536.9139168</v>
+        <v>-383760536.9139168</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -4187,7 +4187,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>171459306.1949863</v>
+        <v>-171459306.1949863</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -4228,7 +4228,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>983563.567887347</v>
+        <v>-983563.567887347</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -4259,16 +4259,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>6933196.386210396</v>
+        <v>-6933196.386210396</v>
       </c>
       <c r="C4">
-        <v>2857808.436630354</v>
+        <v>-2857808.436630354</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>450100867.976267</v>
+        <v>-450100867.976267</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -4282,7 +4282,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>208946965.1671603</v>
+        <v>-208946965.1671603</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -4323,7 +4323,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>848789.7361658283</v>
+        <v>-848789.7361658283</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -4354,16 +4354,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>8358560.6359403</v>
+        <v>-8358560.6359403</v>
       </c>
       <c r="C4">
-        <v>2466214.23173513</v>
+        <v>-2466214.23173513</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>542549081.6943617</v>
+        <v>-542549081.6943617</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -4377,7 +4377,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>256396357.2994952</v>
+        <v>-256396357.2994952</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -4418,7 +4418,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>737775.668711297</v>
+        <v>-737775.668711297</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -4449,16 +4449,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>11836594.91431821</v>
+        <v>-11836594.91431821</v>
       </c>
       <c r="C4">
-        <v>2143655.579793938</v>
+        <v>-2143655.579793938</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>669631849.7563579</v>
+        <v>-669631849.7563579</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -4472,7 +4472,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>314436339.6259276</v>
+        <v>-314436339.6259276</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -4513,7 +4513,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>929562.0123908296</v>
+        <v>-929562.0123908296</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -4544,16 +4544,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>18221565.10305817</v>
+        <v>-18221565.10305817</v>
       </c>
       <c r="C4">
-        <v>2700903.376370145</v>
+        <v>-2700903.376370145</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>844088441.2751006</v>
+        <v>-844088441.2751006</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -4567,7 +4567,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>382915820.7367338</v>
+        <v>-382915820.7367338</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -4608,7 +4608,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>1435124.260485362</v>
+        <v>-1435124.260485362</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -4639,16 +4639,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>26946149.32545647</v>
+        <v>-26946149.32545647</v>
       </c>
       <c r="C4">
-        <v>4169847.636830843</v>
+        <v>-4169847.636830843</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>1060107261.959167</v>
+        <v>-1060107261.959167</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -4662,7 +4662,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>460763881.9920723</v>
+        <v>-460763881.9920723</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -4703,7 +4703,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>1993895.763585281</v>
+        <v>-1993895.763585281</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -4734,16 +4734,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>36542711.27256908</v>
+        <v>-36542711.27256908</v>
       </c>
       <c r="C4">
-        <v>5793394.876525341</v>
+        <v>-5793394.876525341</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>1296919384.28615</v>
+        <v>-1296919384.28615</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -4757,7 +4757,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>545913060.9877158</v>
+        <v>-545913060.9877158</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -4798,7 +4798,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>2806577.173897451</v>
+        <v>-2806577.173897451</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -4829,16 +4829,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>50804721.49013367</v>
+        <v>-50804721.49013367</v>
       </c>
       <c r="C4">
-        <v>8154693.999947914</v>
+        <v>-8154693.999947914</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>1581638408.802744</v>
+        <v>-1581638408.802744</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -4852,7 +4852,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>635295142.5534112</v>
+        <v>-635295142.5534112</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -4933,7 +4933,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>19.54962627494258</v>
+        <v>-19.54962627494258</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -4947,7 +4947,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>10.87747718898359</v>
+        <v>-10.87747718898359</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -4988,7 +4988,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>3873684.383499886</v>
+        <v>-3873684.383499886</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -5019,16 +5019,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>69766226.99399781</v>
+        <v>-69766226.99399781</v>
       </c>
       <c r="C4">
-        <v>11255243.96535717</v>
+        <v>-11255243.96535717</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>1907366730.604346</v>
+        <v>-1907366730.604346</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -5042,7 +5042,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>724926659.4494559</v>
+        <v>-724926659.4494559</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -5083,7 +5083,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>4417286.682874602</v>
+        <v>-4417286.682874602</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -5114,16 +5114,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>79506960.66209157</v>
+        <v>-79506960.66209157</v>
       </c>
       <c r="C4">
-        <v>12834716.08901624</v>
+        <v>-12834716.08901624</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>2144924433.539755</v>
+        <v>-2144924433.539755</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -5137,7 +5137,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>810107908.7226939</v>
+        <v>-810107908.7226939</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -5178,7 +5178,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>4454803.220586355</v>
+        <v>-4454803.220586355</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -5209,16 +5209,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>79975813.56225874</v>
+        <v>-79975813.56225874</v>
       </c>
       <c r="C4">
-        <v>12943722.84921589</v>
+        <v>-12943722.84921589</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>2285218502.570972</v>
+        <v>-2285218502.570972</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -5232,7 +5232,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>885752939.6604817</v>
+        <v>-885752939.6604817</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -5273,7 +5273,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>4418330.190308928</v>
+        <v>-4418330.190308928</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -5304,16 +5304,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>78950068.64845344</v>
+        <v>-78950068.64845344</v>
       </c>
       <c r="C4">
-        <v>12837748.0682872</v>
+        <v>-12837748.0682872</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>2386621675.208046</v>
+        <v>-2386621675.208046</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -5327,7 +5327,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>946843085.1494324</v>
+        <v>-946843085.1494324</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -5368,7 +5368,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>4304981.093526039</v>
+        <v>-4304981.093526039</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -5399,16 +5399,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>76629167.90322736</v>
+        <v>-76629167.90322736</v>
       </c>
       <c r="C4">
-        <v>12508404.83552965</v>
+        <v>-12508404.83552965</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>2442580496.181271</v>
+        <v>-2442580496.181271</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -5422,7 +5422,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>988958596.933805</v>
+        <v>-988958596.933805</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -5463,7 +5463,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>4131553.33053973</v>
+        <v>-4131553.33053973</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -5494,16 +5494,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>73272715.54569723</v>
+        <v>-73272715.54569723</v>
       </c>
       <c r="C4">
-        <v>12004499.09888999</v>
+        <v>-12004499.09888999</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>2449483328.41453</v>
+        <v>-2449483328.41453</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -5517,7 +5517,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>1008806299.391212</v>
+        <v>-1008806299.391212</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -5558,7 +5558,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>3999514.308744036</v>
+        <v>-3999514.308744036</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -5589,16 +5589,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>70594663.51669756</v>
+        <v>-70594663.51669756</v>
       </c>
       <c r="C4">
-        <v>11620851.06354981</v>
+        <v>-11620851.06354981</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>2419199907.429399</v>
+        <v>-2419199907.429399</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -5612,7 +5612,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>1004642776.440383</v>
+        <v>-1004642776.440383</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -5653,7 +5653,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>3844420.933452066</v>
+        <v>-3844420.933452066</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -5684,16 +5684,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>67314160.37668839</v>
+        <v>-67314160.37668839</v>
       </c>
       <c r="C4">
-        <v>11170217.09250217</v>
+        <v>-11170217.09250217</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>2340858819.375082</v>
+        <v>-2340858819.375082</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -5707,7 +5707,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>976504100.799594</v>
+        <v>-976504100.799594</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -5748,7 +5748,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>3454856.110883066</v>
+        <v>-3454856.110883066</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -5779,16 +5779,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>59480235.56764472</v>
+        <v>-59480235.56764472</v>
       </c>
       <c r="C4">
-        <v>10038310.95760595</v>
+        <v>-10038310.95760595</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>2183663649.213801</v>
+        <v>-2183663649.213801</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -5802,7 +5802,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>926195219.963576</v>
+        <v>-926195219.963576</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -5843,7 +5843,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>2602311.781942395</v>
+        <v>-2602311.781942395</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -5874,16 +5874,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>43080183.125532</v>
+        <v>-43080183.125532</v>
       </c>
       <c r="C4">
-        <v>7561187.510382999</v>
+        <v>-7561187.510382999</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>1918703856.76227</v>
+        <v>-1918703856.76227</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -5897,7 +5897,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>857052120.9182549</v>
+        <v>-857052120.9182549</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -5978,7 +5978,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>94.25061177621188</v>
+        <v>-94.25061177621188</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -5992,7 +5992,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>52.44135438832086</v>
+        <v>-52.44135438832086</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -6033,7 +6033,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>1407769.086697244</v>
+        <v>-1407769.086697244</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -6064,16 +6064,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>20979586.27255673</v>
+        <v>-20979586.27255673</v>
       </c>
       <c r="C4">
-        <v>4090365.385769945</v>
+        <v>-4090365.385769945</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>1577917166.187736</v>
+        <v>-1577917166.187736</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -6087,7 +6087,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>773544020.8281935</v>
+        <v>-773544020.8281935</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -6128,7 +6128,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>743679.6293205353</v>
+        <v>-743679.6293205353</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -6159,16 +6159,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>9491948.649370216</v>
+        <v>-9491948.649370216</v>
       </c>
       <c r="C4">
-        <v>2160809.924453996</v>
+        <v>-2160809.924453996</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>1311076790.028383</v>
+        <v>-1311076790.028383</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -6182,7 +6182,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>680808065.8843236</v>
+        <v>-680808065.8843236</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -6223,7 +6223,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>581676.7599233914</v>
+        <v>-581676.7599233914</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -6254,16 +6254,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>8117557.660507199</v>
+        <v>-8117557.660507199</v>
       </c>
       <c r="C4">
-        <v>1690099.965243194</v>
+        <v>-1690099.965243194</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>1123454081.349782</v>
+        <v>-1123454081.349782</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -6277,7 +6277,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>584194701.2707564</v>
+        <v>-584194701.2707564</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -6318,7 +6318,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>405029.635980593</v>
+        <v>-405029.635980593</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -6349,16 +6349,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>7005882.310030884</v>
+        <v>-7005882.310030884</v>
       </c>
       <c r="C4">
-        <v>1176840.164257929</v>
+        <v>-1176840.164257929</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>939696375.8688031</v>
+        <v>-939696375.8688031</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -6372,7 +6372,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>488859189.5829946</v>
+        <v>-488859189.5829946</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -6413,7 +6413,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>226809.9605518837</v>
+        <v>-226809.9605518837</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -6444,16 +6444,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>4900414.185365514</v>
+        <v>-4900414.185365514</v>
       </c>
       <c r="C4">
-        <v>659011.2118215534</v>
+        <v>-659011.2118215534</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>759177872.3736604</v>
+        <v>-759177872.3736604</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -6467,7 +6467,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>399394649.3594545</v>
+        <v>-399394649.3594545</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -6508,7 +6508,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>81783.4671562896</v>
+        <v>-81783.4671562896</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -6539,16 +6539,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>2390836.606113592</v>
+        <v>-2390836.606113592</v>
       </c>
       <c r="C4">
-        <v>237627.2261874744</v>
+        <v>-237627.2261874744</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>593696201.5495499</v>
+        <v>-593696201.5495499</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -6562,7 +6562,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>319495218.7495701</v>
+        <v>-319495218.7495701</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -6603,7 +6603,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>28228.62141637032</v>
+        <v>-28228.62141637032</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -6634,16 +6634,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>1854442.651077511</v>
+        <v>-1854442.651077511</v>
       </c>
       <c r="C4">
-        <v>82020.11041485344</v>
+        <v>-82020.11041485344</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>466573784.2916272</v>
+        <v>-466573784.2916272</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -6657,7 +6657,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>251670131.7410564</v>
+        <v>-251670131.7410564</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -6698,7 +6698,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>66182.16730041227</v>
+        <v>-66182.16730041227</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -6729,16 +6729,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>3317713.753423617</v>
+        <v>-3317713.753423617</v>
       </c>
       <c r="C4">
-        <v>192296.6265127691</v>
+        <v>-192296.6265127691</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>380077176.1978923</v>
+        <v>-380077176.1978923</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -6752,7 +6752,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>197072159.7964708</v>
+        <v>-197072159.7964708</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -6793,7 +6793,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>168040.9545611475</v>
+        <v>-168040.9545611475</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -6824,16 +6824,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>5434534.685062595</v>
+        <v>-5434534.685062595</v>
       </c>
       <c r="C4">
-        <v>488254.0115589852</v>
+        <v>-488254.0115589852</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>323348729.7090754</v>
+        <v>-323348729.7090754</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -6847,7 +6847,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>155514424.4953961</v>
+        <v>-155514424.4953961</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -6888,7 +6888,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>345151.4220588048</v>
+        <v>-345151.4220588048</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -6919,16 +6919,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>7796640.659392156</v>
+        <v>-7796640.659392156</v>
       </c>
       <c r="C4">
-        <v>1002860.087623327</v>
+        <v>-1002860.087623327</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>291354056.6477976</v>
+        <v>-291354056.6477976</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -6942,7 +6942,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>125705647.5798842</v>
+        <v>-125705647.5798842</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -6983,7 +6983,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>1.589604956863446E-11</v>
+        <v>-1.589604956863446E-11</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -7014,16 +7014,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>1.111783199796901E-08</v>
+        <v>-1.111783199796901E-08</v>
       </c>
       <c r="C4">
-        <v>4.618701429122168E-11</v>
+        <v>-4.618701429122168E-11</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>339.0283052779705</v>
+        <v>-339.0283052779705</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -7037,7 +7037,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>188.6364784844114</v>
+        <v>-188.6364784844114</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -7078,7 +7078,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>540699.4177216593</v>
+        <v>-540699.4177216593</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -7109,16 +7109,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>10003394.90379475</v>
+        <v>-10003394.90379475</v>
       </c>
       <c r="C4">
-        <v>1571037.610680452</v>
+        <v>-1571037.610680452</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>276204656.9120699</v>
+        <v>-276204656.9120699</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -7132,7 +7132,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>105653903.2700934</v>
+        <v>-105653903.2700934</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -7173,7 +7173,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>684216.2990491848</v>
+        <v>-684216.2990491848</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -7204,16 +7204,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>11993264.55469231</v>
+        <v>-11993264.55469231</v>
       </c>
       <c r="C4">
-        <v>1988035.319468762</v>
+        <v>-1988035.319468762</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>271721740.03163</v>
+        <v>-271721740.03163</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -7227,7 +7227,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>93121458.185967</v>
+        <v>-93121458.185967</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -7268,7 +7268,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>765208.9728815601</v>
+        <v>-765208.9728815601</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -7299,16 +7299,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>13473655.20081821</v>
+        <v>-13473655.20081821</v>
       </c>
       <c r="C4">
-        <v>2223364.843802998</v>
+        <v>-2223364.843802998</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>271723735.5221689</v>
+        <v>-271723735.5221689</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -7322,7 +7322,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>86001925.85970795</v>
+        <v>-86001925.85970795</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -7363,7 +7363,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>699163.7179161935</v>
+        <v>-699163.7179161935</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -7394,16 +7394,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>12385481.308461</v>
+        <v>-12385481.308461</v>
       </c>
       <c r="C4">
-        <v>2031466.025056749</v>
+        <v>-2031466.025056749</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>255940875.1563143</v>
+        <v>-255940875.1563143</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -7417,7 +7417,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>82542113.05527678</v>
+        <v>-82542113.05527678</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -7458,7 +7458,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>424696.2880995963</v>
+        <v>-424696.2880995963</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -7489,16 +7489,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>7522271.015940348</v>
+        <v>-7522271.015940348</v>
       </c>
       <c r="C4">
-        <v>1233982.911489493</v>
+        <v>-1233982.911489493</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>211659460.4591112</v>
+        <v>-211659460.4591112</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -7512,7 +7512,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>81408891.40481395</v>
+        <v>-81408891.40481395</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -7553,7 +7553,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>140064.7465576346</v>
+        <v>-140064.7465576346</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -7584,16 +7584,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>2433997.379721509</v>
+        <v>-2433997.379721509</v>
       </c>
       <c r="C4">
-        <v>406967.3048653899</v>
+        <v>-406967.3048653899</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>167966154.950975</v>
+        <v>-167966154.950975</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -7607,7 +7607,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>81656484.83868907</v>
+        <v>-81656484.83868907</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -7648,7 +7648,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>20416.6248915248</v>
+        <v>-20416.6248915248</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -7679,16 +7679,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>324600.9435772256</v>
+        <v>-324600.9435772256</v>
       </c>
       <c r="C4">
-        <v>59321.84229621614</v>
+        <v>-59321.84229621614</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>151425411.3656645</v>
+        <v>-151425411.3656645</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -7702,7 +7702,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>82656469.94793797</v>
+        <v>-82656469.94793797</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -7743,7 +7743,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>4592.64696098905</v>
+        <v>-4592.64696098905</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -7774,16 +7774,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>65604.07518312259</v>
+        <v>-65604.07518312259</v>
       </c>
       <c r="C4">
-        <v>13344.23687507154</v>
+        <v>-13344.23687507154</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>151606482.2141586</v>
+        <v>-151606482.2141586</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -7797,7 +7797,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>84025276.73310132</v>
+        <v>-84025276.73310132</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -7838,7 +7838,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>11040.05552162052</v>
+        <v>-11040.05552162052</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -7869,16 +7869,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>157158.0563873459</v>
+        <v>-157158.0563873459</v>
       </c>
       <c r="C4">
-        <v>32077.60519060653</v>
+        <v>-32077.60519060653</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>155182378.1980187</v>
+        <v>-155182378.1980187</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -7892,7 +7892,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>85555161.68257809</v>
+        <v>-85555161.68257809</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -7933,7 +7933,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>29386.99753444836</v>
+        <v>-29386.99753444836</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -7964,16 +7964,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>420120.4515445815</v>
+        <v>-420120.4515445815</v>
       </c>
       <c r="C4">
-        <v>85385.84817814331</v>
+        <v>-85385.84817814331</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>160409796.4331943</v>
+        <v>-160409796.4331943</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -7987,7 +7987,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>87145508.92558889</v>
+        <v>-87145508.92558889</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -8028,7 +8028,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>1.218444815348187E-09</v>
+        <v>-1.218444815348187E-09</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -8059,16 +8059,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>6.633022240675809E-07</v>
+        <v>-6.633022240675809E-07</v>
       </c>
       <c r="C4">
-        <v>3.54027130178269E-09</v>
+        <v>-3.54027130178269E-09</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>1031.158597295639</v>
+        <v>-1031.158597295639</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -8082,7 +8082,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>573.7400761236222</v>
+        <v>-573.7400761236222</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -8123,7 +8123,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>63548.85589293628</v>
+        <v>-63548.85589293628</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -8154,16 +8154,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>916605.6967384262</v>
+        <v>-916605.6967384262</v>
       </c>
       <c r="C4">
-        <v>184645.3675578199</v>
+        <v>-184645.3675578199</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>167734342.4322678</v>
+        <v>-167734342.4322678</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -8177,7 +8177,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>88738518.32914996</v>
+        <v>-88738518.32914996</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -8218,7 +8218,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>90583.69912319179</v>
+        <v>-90583.69912319179</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -8249,16 +8249,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>1345351.453615279</v>
+        <v>-1345351.453615279</v>
       </c>
       <c r="C4">
-        <v>263196.8771794657</v>
+        <v>-263196.8771794657</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>174282770.0194578</v>
+        <v>-174282770.0194578</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -8272,7 +8272,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>90271615.28376357</v>
+        <v>-90271615.28376357</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -8313,7 +8313,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>68726.46998034776</v>
+        <v>-68726.46998034776</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -8344,16 +8344,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>1177958.203737824</v>
+        <v>-1177958.203737824</v>
       </c>
       <c r="C4">
-        <v>199689.2647737397</v>
+        <v>-199689.2647737397</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>175020430.065585</v>
+        <v>-175020430.065585</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -8367,7 +8367,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>91658328.10485151</v>
+        <v>-91658328.10485151</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -8408,7 +8408,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>77666.70592227115</v>
+        <v>-77666.70592227115</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -8439,16 +8439,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>1674986.275723395</v>
+        <v>-1674986.275723395</v>
       </c>
       <c r="C4">
-        <v>225665.7064949127</v>
+        <v>-225665.7064949127</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>180928136.1109165</v>
+        <v>-180928136.1109165</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -8462,7 +8462,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>92800650.99332076</v>
+        <v>-92800650.99332076</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -8503,7 +8503,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>175622.2056025239</v>
+        <v>-175622.2056025239</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -8534,16 +8534,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>3840353.374815279</v>
+        <v>-3840353.374815279</v>
       </c>
       <c r="C4">
-        <v>510281.8335459211</v>
+        <v>-510281.8335459211</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>200631613.2567949</v>
+        <v>-200631613.2567949</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -8557,7 +8557,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>93624772.18001546</v>
+        <v>-93624772.18001546</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -8598,7 +8598,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>312068.3738927328</v>
+        <v>-312068.3738927328</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -8629,16 +8629,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>6789592.943362529</v>
+        <v>-6789592.943362529</v>
       </c>
       <c r="C4">
-        <v>906735.121992963</v>
+        <v>-906735.121992963</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>226419949.4292308</v>
+        <v>-226419949.4292308</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -8652,7 +8652,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>94123347.5600283</v>
+        <v>-94123347.5600283</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -8693,7 +8693,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>386040.6951581968</v>
+        <v>-386040.6951581968</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -8724,16 +8724,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>8211481.804117569</v>
+        <v>-8211481.804117569</v>
       </c>
       <c r="C4">
-        <v>1121666.551634719</v>
+        <v>-1121666.551634719</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>239088152.192413</v>
+        <v>-239088152.192413</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -8747,7 +8747,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>94384197.3716442</v>
+        <v>-94384197.3716442</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -8788,7 +8788,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>410772.6879294108</v>
+        <v>-410772.6879294108</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -8819,16 +8819,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>8214587.934447562</v>
+        <v>-8214587.934447562</v>
       </c>
       <c r="C4">
-        <v>1193526.978254701</v>
+        <v>-1193526.978254701</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>240078115.6370034</v>
+        <v>-240078115.6370034</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -8842,7 +8842,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>94589104.75993688</v>
+        <v>-94589104.75993688</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -8883,7 +8883,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>452753.6862492844</v>
+        <v>-452753.6862492844</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -8914,16 +8914,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>8539830.709998269</v>
+        <v>-8539830.709998269</v>
       </c>
       <c r="C4">
-        <v>1315505.521476262</v>
+        <v>-1315505.521476262</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>244173246.283282</v>
+        <v>-244173246.283282</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -8937,7 +8937,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>94977323.95180692</v>
+        <v>-94977323.95180692</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -8978,7 +8978,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>507898.4478901185</v>
+        <v>-507898.4478901185</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -9009,16 +9009,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>9431511.683743216</v>
+        <v>-9431511.683743216</v>
       </c>
       <c r="C4">
-        <v>1475732.242146335</v>
+        <v>-1475732.242146335</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>253483962.5425471</v>
+        <v>-253483962.5425471</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -9032,7 +9032,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>95783165.5884576</v>
+        <v>-95783165.5884576</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -9073,7 +9073,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>4.62009344937217E-08</v>
+        <v>-4.62009344937217E-08</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -9104,16 +9104,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>2.10290468668763E-05</v>
+        <v>-2.10290468668763E-05</v>
       </c>
       <c r="C4">
-        <v>1.342398444667552E-07</v>
+        <v>-1.342398444667552E-07</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>2767.200005902752</v>
+        <v>-2767.200005902752</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -9127,7 +9127,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>1539.679215945937</v>
+        <v>-1539.679215945937</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -9168,7 +9168,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>557913.9625220244</v>
+        <v>-557913.9625220244</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -9199,16 +9199,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>10228954.48471763</v>
+        <v>-10228954.48471763</v>
       </c>
       <c r="C4">
-        <v>1621055.599318345</v>
+        <v>-1621055.599318345</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>263023190.8231534</v>
+        <v>-263023190.8231534</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -9222,7 +9222,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>97169077.53933673</v>
+        <v>-97169077.53933673</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -9263,7 +9263,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>602469.3850404047</v>
+        <v>-602469.3850404047</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -9294,16 +9294,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>10619732.93516606</v>
+        <v>-10619732.93516606</v>
       </c>
       <c r="C4">
-        <v>1750514.300848088</v>
+        <v>-1750514.300848088</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>270574113.30704</v>
+        <v>-270574113.30704</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -9317,7 +9317,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>99178509.69583741</v>
+        <v>-99178509.69583741</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -9358,7 +9358,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>630603.1249206397</v>
+        <v>-630603.1249206397</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -9389,16 +9389,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>10642842.07226572</v>
+        <v>-10642842.07226572</v>
       </c>
       <c r="C4">
-        <v>1832258.726738523</v>
+        <v>-1832258.726738523</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>276000284.2174075</v>
+        <v>-276000284.2174075</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -9412,7 +9412,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>101724432.0752617</v>
+        <v>-101724432.0752617</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -9453,7 +9453,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>613962.0657685545</v>
+        <v>-613962.0657685545</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -9484,16 +9484,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>10232800.12343889</v>
+        <v>-10232800.12343889</v>
       </c>
       <c r="C4">
-        <v>1783907.03825392</v>
+        <v>-1783907.03825392</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>277789432.4876958</v>
+        <v>-277789432.4876958</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -9507,7 +9507,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>104614158.8296358</v>
+        <v>-104614158.8296358</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -9548,7 +9548,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>543049.418072309</v>
+        <v>-543049.418072309</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -9579,16 +9579,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>9276538.239870105</v>
+        <v>-9276538.239870105</v>
       </c>
       <c r="C4">
-        <v>1577865.6907837</v>
+        <v>-1577865.6907837</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>274434227.4925404</v>
+        <v>-274434227.4925404</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -9602,7 +9602,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>107597476.6360729</v>
+        <v>-107597476.6360729</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -9643,7 +9643,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>432018.2048006595</v>
+        <v>-432018.2048006595</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -9674,16 +9674,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>7635501.086142983</v>
+        <v>-7635501.086142983</v>
       </c>
       <c r="C4">
-        <v>1255257.220546658</v>
+        <v>-1255257.220546658</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>264805146.9058208</v>
+        <v>-264805146.9058208</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -9697,7 +9697,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>110419507.5106448</v>
+        <v>-110419507.5106448</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -9738,7 +9738,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>312003.1987706858</v>
+        <v>-312003.1987706858</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -9769,16 +9769,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>5613997.473699126</v>
+        <v>-5613997.473699126</v>
       </c>
       <c r="C4">
-        <v>906545.7514024638</v>
+        <v>-906545.7514024638</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>251493409.7523204</v>
+        <v>-251493409.7523204</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -9792,7 +9792,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>112863099.9737142</v>
+        <v>-112863099.9737142</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -9833,7 +9833,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>231756.4985792394</v>
+        <v>-231756.4985792394</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -9864,16 +9864,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>4172817.009371918</v>
+        <v>-4172817.009371918</v>
       </c>
       <c r="C4">
-        <v>673383.702393824</v>
+        <v>-673383.702393824</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>242434457.1434241</v>
+        <v>-242434457.1434241</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -9887,7 +9887,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>114773565.6374322</v>
+        <v>-114773565.6374322</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -9928,7 +9928,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>241214.3252514791</v>
+        <v>-241214.3252514791</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -9959,16 +9959,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>4322846.111144232</v>
+        <v>-4322846.111144232</v>
       </c>
       <c r="C4">
-        <v>700864.0379192347</v>
+        <v>-700864.0379192347</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>246084678.4321258</v>
+        <v>-246084678.4321258</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -9982,7 +9982,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>116066085.2723745</v>
+        <v>-116066085.2723745</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -10023,7 +10023,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>315487.1441524533</v>
+        <v>-315487.1441524533</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -10054,16 +10054,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>5643299.520138223</v>
+        <v>-5643299.520138223</v>
       </c>
       <c r="C4">
-        <v>916668.5831439452</v>
+        <v>-916668.5831439452</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>258724611.4385369</v>
+        <v>-258724611.4385369</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -10077,7 +10077,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>116720278.6975065</v>
+        <v>-116720278.6975065</v>
       </c>
       <c r="E5">
         <v>0</v>

</xml_diff>